<commit_message>
Updated status, performed by
</commit_message>
<xml_diff>
--- a/docs/Shedule_Work_breakdown.xlsx
+++ b/docs/Shedule_Work_breakdown.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Complete-EB</t>
+  </si>
+  <si>
+    <t>Complete-AK</t>
   </si>
 </sst>
 </file>
@@ -774,11 +777,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="49681152"/>
-        <c:axId val="49682688"/>
+        <c:axId val="125388672"/>
+        <c:axId val="125390208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49681152"/>
+        <c:axId val="125388672"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -787,7 +790,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49682688"/>
+        <c:crossAx val="125390208"/>
         <c:crossesAt val="41340"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -795,7 +798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49682688"/>
+        <c:axId val="125390208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="41411"/>
@@ -819,7 +822,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49681152"/>
+        <c:crossAx val="125388672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -1163,7 +1166,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1171,6 +1174,7 @@
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1205,7 +1209,7 @@
         <v>41368</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1223,7 +1227,7 @@
         <v>41368</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1241,7 +1245,7 @@
         <v>41370</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1259,7 +1263,7 @@
         <v>41372</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1277,7 +1281,7 @@
         <v>41371</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1295,7 +1299,7 @@
         <v>41375</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1313,7 +1317,7 @@
         <v>41372</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1331,7 +1335,7 @@
         <v>41374</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1439,7 +1443,7 @@
         <v>41379</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1457,7 +1461,7 @@
         <v>41379</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1529,7 +1533,7 @@
         <v>41383</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1546,6 +1550,9 @@
         <f t="shared" si="0"/>
         <v>41383</v>
       </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1561,6 +1568,9 @@
         <f t="shared" si="0"/>
         <v>41390</v>
       </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1576,6 +1586,9 @@
         <f t="shared" si="0"/>
         <v>41390</v>
       </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1591,6 +1604,9 @@
         <f t="shared" si="0"/>
         <v>41397</v>
       </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1605,6 +1621,9 @@
       <c r="D25" s="1">
         <f t="shared" si="0"/>
         <v>41404</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>